<commit_message>
changed headers for test files
</commit_message>
<xml_diff>
--- a/public/no.xlsx
+++ b/public/no.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jk\Desktop\gpt\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{331E0802-035A-457D-83C1-D877A4B2E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DCC317-39EC-47A6-ADDC-7993EA1D6B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="2055" windowWidth="26955" windowHeight="18330" xr2:uid="{F94E33A1-D4EC-42FB-AF72-6770090435C9}"/>
+    <workbookView xWindow="13305" yWindow="2400" windowWidth="26955" windowHeight="18330" xr2:uid="{F94E33A1-D4EC-42FB-AF72-6770090435C9}"/>
   </bookViews>
   <sheets>
     <sheet name="no" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name </t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>https://www.cungu.com/</t>
   </si>
   <si>
@@ -170,6 +161,15 @@
   </si>
   <si>
     <t>A4377097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company name </t>
+  </si>
+  <si>
+    <t>Record ID</t>
+  </si>
+  <si>
+    <t>Website URL</t>
   </si>
 </sst>
 </file>
@@ -1033,28 +1033,33 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>45935689</v>
@@ -1062,167 +1067,167 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>